<commit_message>
decoder with temp, hum, co2
</commit_message>
<xml_diff>
--- a/2 Decoder RoomSensor/decoder helper.xlsx
+++ b/2 Decoder RoomSensor/decoder helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tintsch/Daten/Job/STFW/STFW IoT/Code/2 Decoder RoomSensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A65604-E3A2-EB4C-AD1B-6AE705CCDE3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43EAF95-1B38-B54C-9A76-4DC0DE1C6C32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="3860" windowWidth="34500" windowHeight="21740" xr2:uid="{B3433464-5F9E-8147-AE2C-DBF6298C40EE}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="28580" windowHeight="20080" xr2:uid="{B3433464-5F9E-8147-AE2C-DBF6298C40EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Decoder</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Byte 14</t>
   </si>
   <si>
-    <t>Byte 15</t>
-  </si>
-  <si>
     <t>Temperature:</t>
   </si>
   <si>
@@ -106,14 +103,48 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Länge</t>
+  </si>
+  <si>
+    <t>Temperatur</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Feucht:</t>
+  </si>
+  <si>
+    <t>CO2:</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Typ CO2</t>
+  </si>
+  <si>
+    <t>Typ t/h</t>
+  </si>
+  <si>
+    <t>be</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00"/>
+    <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -138,12 +169,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -168,6 +217,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D13E167-E36C-AB4B-B9D0-864547B33173}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,77 +611,187 @@
       <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4">
-        <v>84</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>40</v>
+      </c>
+      <c r="G4" s="11">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11">
         <v>2</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="I4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13">
+        <v>5</v>
+      </c>
+      <c r="L4" s="13">
+        <v>3</v>
+      </c>
+      <c r="M4" s="13">
+        <v>2</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>E4&amp;D4</f>
-        <v>284</v>
+        <v>918</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E8" s="4">
+        <f>F4</f>
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="9" t="str">
+        <f>J4&amp;I4</f>
+        <v>1EA</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <f>HEX2DEC(E4&amp;D4)</f>
-        <v>644</v>
+        <v>2328</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <f>HEX2DEC(E8)</f>
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9">
+        <f>HEX2DEC(I8)</f>
+        <v>490</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3">
         <v>0.01</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7">
         <f>B9*B10</f>
-        <v>6.44</v>
+        <v>23.28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
+        <f>E9*E10</f>
+        <v>32</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1">
+        <f>I9*I10</f>
+        <v>490</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D5:E5"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed decoder from examples file, updated Excel-sheet
</commit_message>
<xml_diff>
--- a/2 Decoder RoomSensor/decoder helper.xlsx
+++ b/2 Decoder RoomSensor/decoder helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tintsch/Daten/Job/STFW/STFW IoT/Code/2 Decoder RoomSensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43EAF95-1B38-B54C-9A76-4DC0DE1C6C32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04A50C-1B69-AD47-981F-D74EC8522E88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="28580" windowHeight="20080" xr2:uid="{B3433464-5F9E-8147-AE2C-DBF6298C40EE}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="24200" windowHeight="20500" xr2:uid="{B3433464-5F9E-8147-AE2C-DBF6298C40EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Decoder</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>be</t>
+  </si>
+  <si>
+    <t>Typ Strom</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="L4" sqref="L4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,6 +686,12 @@
       <c r="H5" t="s">
         <v>31</v>
       </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>